<commit_message>
momentum's convoluted batch calls done
</commit_message>
<xml_diff>
--- a/output/rec-equal-weight.xlsx
+++ b/output/rec-equal-weight.xlsx
@@ -1942,7 +1942,7 @@
         <v>44896766381</v>
       </c>
       <c r="D2">
-        <v>130</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1956,7 +1956,7 @@
         <v>10918334902</v>
       </c>
       <c r="D3">
-        <v>1178</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1970,7 +1970,7 @@
         <v>9095288378</v>
       </c>
       <c r="D4">
-        <v>130</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1984,7 +1984,7 @@
         <v>2457622872180</v>
       </c>
       <c r="D5">
-        <v>127</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1998,7 +1998,7 @@
         <v>267146665538</v>
       </c>
       <c r="D6">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2012,7 +2012,7 @@
         <v>32120622836</v>
       </c>
       <c r="D7">
-        <v>124</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2026,7 +2026,7 @@
         <v>17180642928</v>
       </c>
       <c r="D8">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2040,7 +2040,7 @@
         <v>187050594797</v>
       </c>
       <c r="D9">
-        <v>184</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2054,7 +2054,7 @@
         <v>189385455764</v>
       </c>
       <c r="D10">
-        <v>68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2068,7 +2068,7 @@
         <v>172105332000</v>
       </c>
       <c r="D11">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2082,7 +2082,7 @@
         <v>99425490446</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2096,7 +2096,7 @@
         <v>44902579715</v>
       </c>
       <c r="D13">
-        <v>242</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2110,7 +2110,7 @@
         <v>94409998845</v>
       </c>
       <c r="D14">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2124,7 +2124,7 @@
         <v>49471171024</v>
       </c>
       <c r="D15">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2138,7 +2138,7 @@
         <v>22188957765</v>
       </c>
       <c r="D16">
-        <v>230</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2152,7 +2152,7 @@
         <v>46720485604</v>
       </c>
       <c r="D17">
-        <v>217</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2166,7 +2166,7 @@
         <v>17827579575</v>
       </c>
       <c r="D18">
-        <v>741</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2180,7 +2180,7 @@
         <v>43071293551</v>
       </c>
       <c r="D19">
-        <v>285</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2194,7 +2194,7 @@
         <v>45938454018</v>
       </c>
       <c r="D20">
-        <v>320</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2208,7 +2208,7 @@
         <v>1153920882</v>
       </c>
       <c r="D21">
-        <v>2602</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2222,7 +2222,7 @@
         <v>6971107057</v>
       </c>
       <c r="D22">
-        <v>150</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2236,7 +2236,7 @@
         <v>40129177200</v>
       </c>
       <c r="D23">
-        <v>104</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2250,7 +2250,7 @@
         <v>12367892477</v>
       </c>
       <c r="D24">
-        <v>251</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2264,7 +2264,7 @@
         <v>31958110675</v>
       </c>
       <c r="D25">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2278,7 +2278,7 @@
         <v>26432438455</v>
       </c>
       <c r="D26">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2292,7 +2292,7 @@
         <v>6376137764</v>
       </c>
       <c r="D27">
-        <v>393</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2306,7 +2306,7 @@
         <v>36373493074</v>
       </c>
       <c r="D28">
-        <v>144</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2320,7 +2320,7 @@
         <v>10680173459</v>
       </c>
       <c r="D29">
-        <v>162</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2334,7 +2334,7 @@
         <v>40336009475</v>
       </c>
       <c r="D30">
-        <v>108</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2348,7 +2348,7 @@
         <v>100714123325</v>
       </c>
       <c r="D31">
-        <v>165</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2362,7 +2362,7 @@
         <v>17101327432</v>
       </c>
       <c r="D32">
-        <v>1720</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2376,7 +2376,7 @@
         <v>137340497879</v>
       </c>
       <c r="D33">
-        <v>232</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2390,7 +2390,7 @@
         <v>33575472841</v>
       </c>
       <c r="D34">
-        <v>135</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2404,7 +2404,7 @@
         <v>128093692088</v>
       </c>
       <c r="D35">
-        <v>82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2418,7 +2418,7 @@
         <v>37277944810</v>
       </c>
       <c r="D36">
-        <v>56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2432,7 +2432,7 @@
         <v>100850173610</v>
       </c>
       <c r="D37">
-        <v>91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2446,7 +2446,7 @@
         <v>1036612797018</v>
       </c>
       <c r="D38">
-        <v>195</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2460,7 +2460,7 @@
         <v>43247692342</v>
       </c>
       <c r="D39">
-        <v>139</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2474,7 +2474,7 @@
         <v>24208490106</v>
       </c>
       <c r="D40">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2488,7 +2488,7 @@
         <v>116342693132</v>
       </c>
       <c r="D41">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2502,7 +2502,7 @@
         <v>65173154546</v>
       </c>
       <c r="D42">
-        <v>62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2516,7 +2516,7 @@
         <v>10393319102</v>
       </c>
       <c r="D43">
-        <v>291</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2530,7 +2530,7 @@
         <v>13281652499</v>
       </c>
       <c r="D44">
-        <v>479</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2544,7 +2544,7 @@
         <v>63173687795</v>
       </c>
       <c r="D45">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2558,7 +2558,7 @@
         <v>48436483710</v>
       </c>
       <c r="D46">
-        <v>243</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2572,7 +2572,7 @@
         <v>33345764688</v>
       </c>
       <c r="D47">
-        <v>160</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2586,7 +2586,7 @@
         <v>28628604190</v>
       </c>
       <c r="D48">
-        <v>119</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2600,7 +2600,7 @@
         <v>16631189948</v>
       </c>
       <c r="D49">
-        <v>170</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2614,7 +2614,7 @@
         <v>60809987286</v>
       </c>
       <c r="D50">
-        <v>254</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2628,7 +2628,7 @@
         <v>25341006160</v>
       </c>
       <c r="D51">
-        <v>109</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2642,7 +2642,7 @@
         <v>253945228417</v>
       </c>
       <c r="D52">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2656,7 +2656,7 @@
         <v>15030278069</v>
       </c>
       <c r="D53">
-        <v>106</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2670,7 +2670,7 @@
         <v>27137810195</v>
       </c>
       <c r="D54">
-        <v>132</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2684,7 +2684,7 @@
         <v>135002531186</v>
       </c>
       <c r="D55">
-        <v>109</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2698,7 +2698,7 @@
         <v>48420497911</v>
       </c>
       <c r="D56">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2712,7 +2712,7 @@
         <v>130081215362</v>
       </c>
       <c r="D57">
-        <v>91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2726,7 +2726,7 @@
         <v>285277690419</v>
       </c>
       <c r="D58">
-        <v>556</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2740,7 +2740,7 @@
         <v>20195077606</v>
       </c>
       <c r="D59">
-        <v>494</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2754,7 +2754,7 @@
         <v>19681473183</v>
       </c>
       <c r="D60">
-        <v>222</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2768,7 +2768,7 @@
         <v>69144244909</v>
       </c>
       <c r="D61">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2782,7 +2782,7 @@
         <v>15878190570</v>
       </c>
       <c r="D62">
-        <v>623</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2796,7 +2796,7 @@
         <v>31405476876</v>
       </c>
       <c r="D63">
-        <v>301</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2810,7 +2810,7 @@
         <v>40173511688</v>
       </c>
       <c r="D64">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2824,7 +2824,7 @@
         <v>13428024986</v>
       </c>
       <c r="D65">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2838,7 +2838,7 @@
         <v>41844652960</v>
       </c>
       <c r="D66">
-        <v>382</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2852,7 +2852,7 @@
         <v>97616598053</v>
       </c>
       <c r="D67">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2866,7 +2866,7 @@
         <v>32197181700</v>
       </c>
       <c r="D68">
-        <v>615</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2880,7 +2880,7 @@
         <v>108770134908</v>
       </c>
       <c r="D69">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2894,7 +2894,7 @@
         <v>22222129619</v>
       </c>
       <c r="D70">
-        <v>284</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2908,7 +2908,7 @@
         <v>151956680000</v>
       </c>
       <c r="D71">
-        <v>277</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2922,7 +2922,7 @@
         <v>17026648625</v>
       </c>
       <c r="D72">
-        <v>136</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2936,7 +2936,7 @@
         <v>683456293237</v>
       </c>
       <c r="D73">
-        <v>63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2950,7 +2950,7 @@
         <v>67734000526</v>
       </c>
       <c r="D74">
-        <v>418</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2964,7 +2964,7 @@
         <v>11562521063</v>
       </c>
       <c r="D75">
-        <v>401</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2978,7 +2978,7 @@
         <v>11472877371</v>
       </c>
       <c r="D76">
-        <v>270</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2992,7 +2992,7 @@
         <v>100367715412</v>
       </c>
       <c r="D77">
-        <v>382</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -3006,7 +3006,7 @@
         <v>17101215336</v>
       </c>
       <c r="D78">
-        <v>551</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -3020,7 +3020,7 @@
         <v>20245277256</v>
       </c>
       <c r="D79">
-        <v>251</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -3034,7 +3034,7 @@
         <v>37938867602</v>
       </c>
       <c r="D80">
-        <v>435</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -3048,7 +3048,7 @@
         <v>129425806589</v>
       </c>
       <c r="D81">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -3062,7 +3062,7 @@
         <v>88384955848</v>
       </c>
       <c r="D82">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -3076,7 +3076,7 @@
         <v>13635802775</v>
       </c>
       <c r="D83">
-        <v>154</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -3090,7 +3090,7 @@
         <v>28280553636</v>
       </c>
       <c r="D84">
-        <v>221</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -3104,7 +3104,7 @@
         <v>60683016380</v>
       </c>
       <c r="D85">
-        <v>141</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -3118,7 +3118,7 @@
         <v>13573315288</v>
       </c>
       <c r="D86">
-        <v>1624</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -3132,7 +3132,7 @@
         <v>55483154160</v>
       </c>
       <c r="D87">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -3146,7 +3146,7 @@
         <v>28786830593</v>
       </c>
       <c r="D88">
-        <v>93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -3160,7 +3160,7 @@
         <v>13324725645</v>
       </c>
       <c r="D89">
-        <v>161</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -3174,7 +3174,7 @@
         <v>27915791082</v>
       </c>
       <c r="D90">
-        <v>208</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -3188,7 +3188,7 @@
         <v>16678066250</v>
       </c>
       <c r="D91">
-        <v>232</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -3202,7 +3202,7 @@
         <v>21388882653</v>
       </c>
       <c r="D92">
-        <v>455</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -3216,7 +3216,7 @@
         <v>20353252241</v>
       </c>
       <c r="D93">
-        <v>237</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -3230,7 +3230,7 @@
         <v>12380681844</v>
       </c>
       <c r="D94">
-        <v>188</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -3244,7 +3244,7 @@
         <v>61611629940</v>
       </c>
       <c r="D95">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -3258,7 +3258,7 @@
         <v>91287551814</v>
       </c>
       <c r="D96">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3272,7 +3272,7 @@
         <v>19918395510</v>
       </c>
       <c r="D97">
-        <v>156</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3286,7 +3286,7 @@
         <v>60720073067</v>
       </c>
       <c r="D98">
-        <v>272</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3300,7 +3300,7 @@
         <v>18989487181</v>
       </c>
       <c r="D99">
-        <v>128</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -3314,7 +3314,7 @@
         <v>9884288586</v>
       </c>
       <c r="D100">
-        <v>262</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -3328,7 +3328,7 @@
         <v>165824643187</v>
       </c>
       <c r="D101">
-        <v>502</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -3342,7 +3342,7 @@
         <v>67732616296</v>
       </c>
       <c r="D102">
-        <v>105</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3356,7 +3356,7 @@
         <v>45921130872</v>
       </c>
       <c r="D103">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3370,7 +3370,7 @@
         <v>35797141754</v>
       </c>
       <c r="D104">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3384,7 +3384,7 @@
         <v>17757593010</v>
       </c>
       <c r="D105">
-        <v>323</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -3398,7 +3398,7 @@
         <v>41393583558</v>
       </c>
       <c r="D106">
-        <v>270</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -3412,7 +3412,7 @@
         <v>18338372931</v>
       </c>
       <c r="D107">
-        <v>679</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3426,7 +3426,7 @@
         <v>43754107308</v>
       </c>
       <c r="D108">
-        <v>172</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -3440,7 +3440,7 @@
         <v>8892528027</v>
       </c>
       <c r="D109">
-        <v>889</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -3454,7 +3454,7 @@
         <v>17105121667</v>
       </c>
       <c r="D110">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -3468,7 +3468,7 @@
         <v>139123834519</v>
       </c>
       <c r="D111">
-        <v>177</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -3482,7 +3482,7 @@
         <v>226869781526</v>
       </c>
       <c r="D112">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3496,7 +3496,7 @@
         <v>9711066401</v>
       </c>
       <c r="D113">
-        <v>1738</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3510,7 +3510,7 @@
         <v>15257872386</v>
       </c>
       <c r="D114">
-        <v>388</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3524,7 +3524,7 @@
         <v>16595803026</v>
       </c>
       <c r="D115">
-        <v>284</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3538,7 +3538,7 @@
         <v>171100000000</v>
       </c>
       <c r="D116">
-        <v>115</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3552,7 +3552,7 @@
         <v>199073499891</v>
       </c>
       <c r="D117">
-        <v>408</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3566,7 +3566,7 @@
         <v>66583284447</v>
       </c>
       <c r="D118">
-        <v>625</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3580,7 +3580,7 @@
         <v>45183513578</v>
       </c>
       <c r="D119">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3594,7 +3594,7 @@
         <v>12072940000</v>
       </c>
       <c r="D120">
-        <v>1800</v>
+        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3608,7 +3608,7 @@
         <v>34350508515</v>
       </c>
       <c r="D121">
-        <v>296</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3622,7 +3622,7 @@
         <v>44377098120</v>
       </c>
       <c r="D122">
-        <v>318</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3636,7 +3636,7 @@
         <v>13183359916</v>
       </c>
       <c r="D123">
-        <v>190</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3650,7 +3650,7 @@
         <v>113451265779</v>
       </c>
       <c r="D124">
-        <v>224</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3664,7 +3664,7 @@
         <v>326804250659</v>
       </c>
       <c r="D125">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3678,7 +3678,7 @@
         <v>12877584384</v>
       </c>
       <c r="D126">
-        <v>301</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3692,7 +3692,7 @@
         <v>48538280691</v>
       </c>
       <c r="D127">
-        <v>339</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3706,7 +3706,7 @@
         <v>25019169885</v>
       </c>
       <c r="D128">
-        <v>507</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3720,7 +3720,7 @@
         <v>37924868290</v>
       </c>
       <c r="D129">
-        <v>259</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3734,7 +3734,7 @@
         <v>121846278422</v>
       </c>
       <c r="D130">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3748,7 +3748,7 @@
         <v>31489269416</v>
       </c>
       <c r="D131">
-        <v>171</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3762,7 +3762,7 @@
         <v>51902889588</v>
       </c>
       <c r="D132">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3776,7 +3776,7 @@
         <v>16698180265</v>
       </c>
       <c r="D133">
-        <v>135</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3790,7 +3790,7 @@
         <v>34078355955</v>
       </c>
       <c r="D134">
-        <v>199</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3804,7 +3804,7 @@
         <v>187166490311</v>
       </c>
       <c r="D135">
-        <v>77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3818,7 +3818,7 @@
         <v>199560421477</v>
       </c>
       <c r="D136">
-        <v>181</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3832,7 +3832,7 @@
         <v>12449494875</v>
       </c>
       <c r="D137">
-        <v>810</v>
+        <v>8</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3843,7 +3843,7 @@
         <v>24.42</v>
       </c>
       <c r="D138">
-        <v>810</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3857,7 +3857,7 @@
         <v>7647476299</v>
       </c>
       <c r="D139">
-        <v>1374</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3871,7 +3871,7 @@
         <v>32671156108</v>
       </c>
       <c r="D140">
-        <v>174</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3885,7 +3885,7 @@
         <v>33397958960</v>
       </c>
       <c r="D141">
-        <v>132</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3899,7 +3899,7 @@
         <v>21966796715</v>
       </c>
       <c r="D142">
-        <v>126</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3913,7 +3913,7 @@
         <v>42123624019</v>
       </c>
       <c r="D143">
-        <v>331</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3927,7 +3927,7 @@
         <v>12747316378</v>
       </c>
       <c r="D144">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3941,7 +3941,7 @@
         <v>18556648911</v>
       </c>
       <c r="D145">
-        <v>410</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3955,7 +3955,7 @@
         <v>17849298711</v>
       </c>
       <c r="D146">
-        <v>135</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3969,7 +3969,7 @@
         <v>22127272792</v>
       </c>
       <c r="D147">
-        <v>173</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3983,7 +3983,7 @@
         <v>75662517663</v>
       </c>
       <c r="D148">
-        <v>201</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3997,7 +3997,7 @@
         <v>7489112000</v>
       </c>
       <c r="D149">
-        <v>238</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -4011,7 +4011,7 @@
         <v>37411251000</v>
       </c>
       <c r="D150">
-        <v>346</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -4025,7 +4025,7 @@
         <v>6684757672</v>
       </c>
       <c r="D151">
-        <v>674</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -4039,7 +4039,7 @@
         <v>46416638881</v>
       </c>
       <c r="D152">
-        <v>164</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -4053,7 +4053,7 @@
         <v>31290933722</v>
       </c>
       <c r="D153">
-        <v>174</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -4067,7 +4067,7 @@
         <v>26943023670</v>
       </c>
       <c r="D154">
-        <v>398</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -4081,7 +4081,7 @@
         <v>46697560437</v>
       </c>
       <c r="D155">
-        <v>120</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -4095,7 +4095,7 @@
         <v>32363491738</v>
       </c>
       <c r="D156">
-        <v>217</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -4109,7 +4109,7 @@
         <v>26757562539</v>
       </c>
       <c r="D157">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -4123,7 +4123,7 @@
         <v>25852915430</v>
       </c>
       <c r="D158">
-        <v>292</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -4137,7 +4137,7 @@
         <v>90884585000</v>
       </c>
       <c r="D159">
-        <v>77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -4151,7 +4151,7 @@
         <v>10689941529</v>
       </c>
       <c r="D160">
-        <v>222</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -4165,7 +4165,7 @@
         <v>49368960000</v>
       </c>
       <c r="D161">
-        <v>229</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4179,7 +4179,7 @@
         <v>75497171921</v>
       </c>
       <c r="D162">
-        <v>154</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -4193,7 +4193,7 @@
         <v>67298344134</v>
       </c>
       <c r="D163">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -4207,7 +4207,7 @@
         <v>25165620883</v>
       </c>
       <c r="D164">
-        <v>297</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -4221,7 +4221,7 @@
         <v>27822796390</v>
       </c>
       <c r="D165">
-        <v>247</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -4235,7 +4235,7 @@
         <v>15490406907</v>
       </c>
       <c r="D166">
-        <v>82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -4249,7 +4249,7 @@
         <v>10891188960</v>
       </c>
       <c r="D167">
-        <v>401</v>
+        <v>4</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4263,7 +4263,7 @@
         <v>69100375000</v>
       </c>
       <c r="D168">
-        <v>113</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4277,7 +4277,7 @@
         <v>21884667633</v>
       </c>
       <c r="D169">
-        <v>184</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -4291,7 +4291,7 @@
         <v>14082057220</v>
       </c>
       <c r="D170">
-        <v>322</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -4305,7 +4305,7 @@
         <v>48174858082</v>
       </c>
       <c r="D171">
-        <v>254</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -4319,7 +4319,7 @@
         <v>42402972420</v>
       </c>
       <c r="D172">
-        <v>464</v>
+        <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -4333,7 +4333,7 @@
         <v>18073119131</v>
       </c>
       <c r="D173">
-        <v>174</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -4347,7 +4347,7 @@
         <v>17459798487</v>
       </c>
       <c r="D174">
-        <v>170</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4361,7 +4361,7 @@
         <v>21719393411</v>
       </c>
       <c r="D175">
-        <v>122</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -4375,7 +4375,7 @@
         <v>50625214120</v>
       </c>
       <c r="D176">
-        <v>1531</v>
+        <v>15</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -4389,7 +4389,7 @@
         <v>26134913474</v>
       </c>
       <c r="D177">
-        <v>135</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -4403,7 +4403,7 @@
         <v>30299846692</v>
       </c>
       <c r="D178">
-        <v>373</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -4417,7 +4417,7 @@
         <v>561210585170</v>
       </c>
       <c r="D179">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4428,7 +4428,7 @@
         <v>57.62</v>
       </c>
       <c r="D180">
-        <v>343</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4442,7 +4442,7 @@
         <v>60474833451</v>
       </c>
       <c r="D181">
-        <v>468</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4456,7 +4456,7 @@
         <v>53770686706</v>
       </c>
       <c r="D182">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4470,7 +4470,7 @@
         <v>23304660228</v>
       </c>
       <c r="D183">
-        <v>485</v>
+        <v>4</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4484,7 +4484,7 @@
         <v>8870800727</v>
       </c>
       <c r="D184">
-        <v>134</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4498,7 +4498,7 @@
         <v>40023444307</v>
       </c>
       <c r="D185">
-        <v>293</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4512,7 +4512,7 @@
         <v>74768205668</v>
       </c>
       <c r="D186">
-        <v>168</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4526,7 +4526,7 @@
         <v>25465297759</v>
       </c>
       <c r="D187">
-        <v>533</v>
+        <v>5</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4540,7 +4540,7 @@
         <v>7565007314</v>
       </c>
       <c r="D188">
-        <v>345</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -4554,7 +4554,7 @@
         <v>4803073076</v>
       </c>
       <c r="D189">
-        <v>538</v>
+        <v>5</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -4568,7 +4568,7 @@
         <v>15575023807</v>
       </c>
       <c r="D190">
-        <v>93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4582,7 +4582,7 @@
         <v>16254642704</v>
       </c>
       <c r="D191">
-        <v>153</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4596,7 +4596,7 @@
         <v>19144749399</v>
       </c>
       <c r="D192">
-        <v>576</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -4610,7 +4610,7 @@
         <v>19218470678</v>
       </c>
       <c r="D193">
-        <v>533</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -4624,7 +4624,7 @@
         <v>24025964503</v>
       </c>
       <c r="D194">
-        <v>148</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -4638,7 +4638,7 @@
         <v>8939900950</v>
       </c>
       <c r="D195">
-        <v>180</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -4652,7 +4652,7 @@
         <v>6317126863</v>
       </c>
       <c r="D196">
-        <v>1399</v>
+        <v>13</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4666,7 +4666,7 @@
         <v>49069433851</v>
       </c>
       <c r="D197">
-        <v>315</v>
+        <v>3</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -4680,7 +4680,7 @@
         <v>24603825914</v>
       </c>
       <c r="D198">
-        <v>284</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -4694,7 +4694,7 @@
         <v>63796754653</v>
       </c>
       <c r="D199">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -4708,7 +4708,7 @@
         <v>92625478228</v>
       </c>
       <c r="D200">
-        <v>233</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -4722,7 +4722,7 @@
         <v>106673439017</v>
       </c>
       <c r="D201">
-        <v>232</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -4736,7 +4736,7 @@
         <v>44285660954</v>
       </c>
       <c r="D202">
-        <v>263</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -4750,7 +4750,7 @@
         <v>11773588518</v>
       </c>
       <c r="D203">
-        <v>163</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4764,7 +4764,7 @@
         <v>30136259327</v>
       </c>
       <c r="D204">
-        <v>555</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -4778,7 +4778,7 @@
         <v>59899668857</v>
       </c>
       <c r="D205">
-        <v>461</v>
+        <v>4</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -4792,7 +4792,7 @@
         <v>1155094154275</v>
       </c>
       <c r="D206">
-        <v>203</v>
+        <v>2</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -4806,7 +4806,7 @@
         <v>1158652714316</v>
       </c>
       <c r="D207">
-        <v>204</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4820,7 +4820,7 @@
         <v>25363871188</v>
       </c>
       <c r="D208">
-        <v>110</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -4834,7 +4834,7 @@
         <v>31896519182</v>
       </c>
       <c r="D209">
-        <v>167</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4848,7 +4848,7 @@
         <v>5109941459</v>
       </c>
       <c r="D210">
-        <v>1409</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4862,7 +4862,7 @@
         <v>18817564942</v>
       </c>
       <c r="D211">
-        <v>201</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -4876,7 +4876,7 @@
         <v>125372419503</v>
       </c>
       <c r="D212">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -4890,7 +4890,7 @@
         <v>33989519342</v>
       </c>
       <c r="D213">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -4904,7 +4904,7 @@
         <v>34311370964</v>
       </c>
       <c r="D214">
-        <v>521</v>
+        <v>5</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -4918,7 +4918,7 @@
         <v>8063079090</v>
       </c>
       <c r="D215">
-        <v>339</v>
+        <v>3</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4932,7 +4932,7 @@
         <v>22232534870</v>
       </c>
       <c r="D216">
-        <v>1285</v>
+        <v>12</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -4946,7 +4946,7 @@
         <v>2078701026</v>
       </c>
       <c r="D217">
-        <v>3328</v>
+        <v>33</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -4960,7 +4960,7 @@
         <v>73234933968</v>
       </c>
       <c r="D218">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -4974,7 +4974,7 @@
         <v>328298833006</v>
       </c>
       <c r="D219">
-        <v>61</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -4988,7 +4988,7 @@
         <v>45016119121</v>
       </c>
       <c r="D220">
-        <v>135</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -5002,7 +5002,7 @@
         <v>5931624949</v>
       </c>
       <c r="D221">
-        <v>544</v>
+        <v>5</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -5016,7 +5016,7 @@
         <v>24748096676</v>
       </c>
       <c r="D222">
-        <v>254</v>
+        <v>2</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -5030,7 +5030,7 @@
         <v>8715331298</v>
       </c>
       <c r="D223">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -5044,7 +5044,7 @@
         <v>41314861157</v>
       </c>
       <c r="D224">
-        <v>129</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -5058,7 +5058,7 @@
         <v>20616847654</v>
       </c>
       <c r="D225">
-        <v>236</v>
+        <v>2</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -5072,7 +5072,7 @@
         <v>135614117417</v>
       </c>
       <c r="D226">
-        <v>98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -5086,7 +5086,7 @@
         <v>21239705221</v>
       </c>
       <c r="D227">
-        <v>1195</v>
+        <v>11</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -5100,7 +5100,7 @@
         <v>29984911152</v>
       </c>
       <c r="D228">
-        <v>648</v>
+        <v>6</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -5114,7 +5114,7 @@
         <v>6046923204</v>
       </c>
       <c r="D229">
-        <v>498</v>
+        <v>4</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -5128,7 +5128,7 @@
         <v>24665588117</v>
       </c>
       <c r="D230">
-        <v>438</v>
+        <v>4</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -5142,7 +5142,7 @@
         <v>12014937048</v>
       </c>
       <c r="D231">
-        <v>223</v>
+        <v>2</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -5156,7 +5156,7 @@
         <v>13177961635</v>
       </c>
       <c r="D232">
-        <v>1074</v>
+        <v>10</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -5170,7 +5170,7 @@
         <v>48487884720</v>
       </c>
       <c r="D233">
-        <v>83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -5184,7 +5184,7 @@
         <v>63087470466</v>
       </c>
       <c r="D234">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -5198,7 +5198,7 @@
         <v>17959239526</v>
       </c>
       <c r="D235">
-        <v>456</v>
+        <v>4</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -5212,7 +5212,7 @@
         <v>123322835913</v>
       </c>
       <c r="D236">
-        <v>145</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -5226,7 +5226,7 @@
         <v>60713599583</v>
       </c>
       <c r="D237">
-        <v>182</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -5240,7 +5240,7 @@
         <v>42616777903</v>
       </c>
       <c r="D238">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -5254,7 +5254,7 @@
         <v>17152268609</v>
       </c>
       <c r="D239">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -5268,7 +5268,7 @@
         <v>24693094203</v>
       </c>
       <c r="D240">
-        <v>204</v>
+        <v>2</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -5282,7 +5282,7 @@
         <v>33670065000</v>
       </c>
       <c r="D241">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -5296,7 +5296,7 @@
         <v>17692274178</v>
       </c>
       <c r="D242">
-        <v>249</v>
+        <v>2</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -5310,7 +5310,7 @@
         <v>45801486922</v>
       </c>
       <c r="D243">
-        <v>182</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -5324,7 +5324,7 @@
         <v>119352450000</v>
       </c>
       <c r="D244">
-        <v>686</v>
+        <v>6</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -5338,7 +5338,7 @@
         <v>118336994434</v>
       </c>
       <c r="D245">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -5352,7 +5352,7 @@
         <v>13806220574</v>
       </c>
       <c r="D246">
-        <v>510</v>
+        <v>5</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -5366,7 +5366,7 @@
         <v>14561906431</v>
       </c>
       <c r="D247">
-        <v>528</v>
+        <v>5</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -5380,7 +5380,7 @@
         <v>6386452465</v>
       </c>
       <c r="D248">
-        <v>151</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -5394,7 +5394,7 @@
         <v>42168557422</v>
       </c>
       <c r="D249">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -5408,7 +5408,7 @@
         <v>23599072302</v>
       </c>
       <c r="D250">
-        <v>339</v>
+        <v>3</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -5422,7 +5422,7 @@
         <v>15483429611</v>
       </c>
       <c r="D251">
-        <v>371</v>
+        <v>3</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -5436,7 +5436,7 @@
         <v>86497941199</v>
       </c>
       <c r="D252">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -5450,7 +5450,7 @@
         <v>27234962323</v>
       </c>
       <c r="D253">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -5464,7 +5464,7 @@
         <v>73740090279</v>
       </c>
       <c r="D254">
-        <v>82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -5478,7 +5478,7 @@
         <v>8540854938</v>
       </c>
       <c r="D255">
-        <v>1054</v>
+        <v>10</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -5492,7 +5492,7 @@
         <v>15557960390</v>
       </c>
       <c r="D256">
-        <v>161</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -5506,7 +5506,7 @@
         <v>19920600185</v>
       </c>
       <c r="D257">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -5520,7 +5520,7 @@
         <v>44806371643</v>
       </c>
       <c r="D258">
-        <v>303</v>
+        <v>3</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -5534,7 +5534,7 @@
         <v>12286873000</v>
       </c>
       <c r="D259">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -5548,7 +5548,7 @@
         <v>416670252448</v>
       </c>
       <c r="D260">
-        <v>124</v>
+        <v>1</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -5562,7 +5562,7 @@
         <v>10229990085</v>
       </c>
       <c r="D261">
-        <v>628</v>
+        <v>6</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -5576,7 +5576,7 @@
         <v>421794862894</v>
       </c>
       <c r="D262">
-        <v>137</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -5590,7 +5590,7 @@
         <v>22848589800</v>
       </c>
       <c r="D263">
-        <v>294</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -5604,7 +5604,7 @@
         <v>17968994361</v>
       </c>
       <c r="D264">
-        <v>1028</v>
+        <v>10</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -5618,7 +5618,7 @@
         <v>33619645160</v>
       </c>
       <c r="D265">
-        <v>105</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -5632,7 +5632,7 @@
         <v>49156447481</v>
       </c>
       <c r="D266">
-        <v>493</v>
+        <v>4</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -5646,7 +5646,7 @@
         <v>0</v>
       </c>
       <c r="D267">
-        <v>929</v>
+        <v>9</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -5660,7 +5660,7 @@
         <v>56009525347</v>
       </c>
       <c r="D268">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -5674,7 +5674,7 @@
         <v>43121364850</v>
       </c>
       <c r="D269">
-        <v>154</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -5688,7 +5688,7 @@
         <v>40891178645</v>
       </c>
       <c r="D270">
-        <v>1088</v>
+        <v>10</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -5702,7 +5702,7 @@
         <v>11938675349</v>
       </c>
       <c r="D271">
-        <v>262</v>
+        <v>2</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -5716,7 +5716,7 @@
         <v>257697745402</v>
       </c>
       <c r="D272">
-        <v>332</v>
+        <v>3</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -5730,7 +5730,7 @@
         <v>31689434406</v>
       </c>
       <c r="D273">
-        <v>447</v>
+        <v>4</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -5744,7 +5744,7 @@
         <v>3695694082</v>
       </c>
       <c r="D274">
-        <v>591</v>
+        <v>5</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -5758,7 +5758,7 @@
         <v>26710947380</v>
       </c>
       <c r="D275">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -5772,7 +5772,7 @@
         <v>14605105377</v>
       </c>
       <c r="D276">
-        <v>318</v>
+        <v>3</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -5786,7 +5786,7 @@
         <v>21957908112</v>
       </c>
       <c r="D277">
-        <v>247</v>
+        <v>2</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -5800,7 +5800,7 @@
         <v>13387375213</v>
       </c>
       <c r="D278">
-        <v>202</v>
+        <v>2</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -5814,7 +5814,7 @@
         <v>4588503710</v>
       </c>
       <c r="D279">
-        <v>572</v>
+        <v>5</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -5828,7 +5828,7 @@
         <v>29373999971</v>
       </c>
       <c r="D280">
-        <v>191</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -5842,7 +5842,7 @@
         <v>21994064000</v>
       </c>
       <c r="D281">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -5856,7 +5856,7 @@
         <v>40607204090</v>
       </c>
       <c r="D282">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -5870,7 +5870,7 @@
         <v>163791222540</v>
       </c>
       <c r="D283">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -5884,7 +5884,7 @@
         <v>15472103381</v>
       </c>
       <c r="D284">
-        <v>341</v>
+        <v>3</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -5898,7 +5898,7 @@
         <v>318319098279</v>
       </c>
       <c r="D285">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -5912,7 +5912,7 @@
         <v>122672904662</v>
       </c>
       <c r="D286">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -5926,7 +5926,7 @@
         <v>5920849085</v>
       </c>
       <c r="D287">
-        <v>565</v>
+        <v>5</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -5940,7 +5940,7 @@
         <v>13414606595</v>
       </c>
       <c r="D288">
-        <v>370</v>
+        <v>3</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -5954,7 +5954,7 @@
         <v>133469242922</v>
       </c>
       <c r="D289">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -5968,7 +5968,7 @@
         <v>70205960181</v>
       </c>
       <c r="D290">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -5982,7 +5982,7 @@
         <v>21227916530</v>
       </c>
       <c r="D291">
-        <v>554</v>
+        <v>5</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -5996,7 +5996,7 @@
         <v>43219659130</v>
       </c>
       <c r="D292">
-        <v>350</v>
+        <v>3</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -6010,7 +6010,7 @@
         <v>14402884765</v>
       </c>
       <c r="D293">
-        <v>197</v>
+        <v>1</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -6024,7 +6024,7 @@
         <v>32598261988</v>
       </c>
       <c r="D294">
-        <v>197</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -6038,7 +6038,7 @@
         <v>18232584045</v>
       </c>
       <c r="D295">
-        <v>250</v>
+        <v>2</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -6052,7 +6052,7 @@
         <v>352713677254</v>
       </c>
       <c r="D296">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -6066,7 +6066,7 @@
         <v>19668045706</v>
       </c>
       <c r="D297">
-        <v>116</v>
+        <v>1</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -6080,7 +6080,7 @@
         <v>57163888712</v>
       </c>
       <c r="D298">
-        <v>109</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -6094,7 +6094,7 @@
         <v>12667970839</v>
       </c>
       <c r="D299">
-        <v>352</v>
+        <v>3</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -6108,7 +6108,7 @@
         <v>195234912652</v>
       </c>
       <c r="D300">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -6122,7 +6122,7 @@
         <v>47061145511</v>
       </c>
       <c r="D301">
-        <v>230</v>
+        <v>2</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -6136,7 +6136,7 @@
         <v>49796580506</v>
       </c>
       <c r="D302">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -6150,7 +6150,7 @@
         <v>56876272000</v>
       </c>
       <c r="D303">
-        <v>63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -6164,7 +6164,7 @@
         <v>89555626911</v>
       </c>
       <c r="D304">
-        <v>301</v>
+        <v>3</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -6178,7 +6178,7 @@
         <v>112386906341</v>
       </c>
       <c r="D305">
-        <v>234</v>
+        <v>2</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -6192,7 +6192,7 @@
         <v>56836873490</v>
       </c>
       <c r="D306">
-        <v>273</v>
+        <v>2</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -6206,7 +6206,7 @@
         <v>16966016677</v>
       </c>
       <c r="D307">
-        <v>448</v>
+        <v>4</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -6220,7 +6220,7 @@
         <v>7510357923</v>
       </c>
       <c r="D308">
-        <v>167</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -6234,7 +6234,7 @@
         <v>20049486398</v>
       </c>
       <c r="D309">
-        <v>264</v>
+        <v>2</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -6248,7 +6248,7 @@
         <v>13493930150</v>
       </c>
       <c r="D310">
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -6262,7 +6262,7 @@
         <v>23768317663</v>
       </c>
       <c r="D311">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -6276,7 +6276,7 @@
         <v>83364317673</v>
       </c>
       <c r="D312">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -6290,7 +6290,7 @@
         <v>62366145000</v>
       </c>
       <c r="D313">
-        <v>174</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -6304,7 +6304,7 @@
         <v>54832644903</v>
       </c>
       <c r="D314">
-        <v>188</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -6318,7 +6318,7 @@
         <v>85397025248</v>
       </c>
       <c r="D315">
-        <v>415</v>
+        <v>4</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -6332,7 +6332,7 @@
         <v>16894668907</v>
       </c>
       <c r="D316">
-        <v>399</v>
+        <v>3</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -6346,7 +6346,7 @@
         <v>59571478483</v>
       </c>
       <c r="D317">
-        <v>155</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -6360,7 +6360,7 @@
         <v>273011438480</v>
       </c>
       <c r="D318">
-        <v>183</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -6374,7 +6374,7 @@
         <v>16506231945</v>
       </c>
       <c r="D319">
-        <v>759</v>
+        <v>7</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -6388,7 +6388,7 @@
         <v>170413732718</v>
       </c>
       <c r="D320">
-        <v>196</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -6402,7 +6402,7 @@
         <v>45230735343</v>
       </c>
       <c r="D321">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -6416,7 +6416,7 @@
         <v>2004765167508</v>
       </c>
       <c r="D322">
-        <v>73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -6430,7 +6430,7 @@
         <v>45480944880</v>
       </c>
       <c r="D323">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -6444,7 +6444,7 @@
         <v>27661288216</v>
       </c>
       <c r="D324">
-        <v>123</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -6458,7 +6458,7 @@
         <v>34819064380</v>
       </c>
       <c r="D325">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -6472,7 +6472,7 @@
         <v>67478357976</v>
       </c>
       <c r="D326">
-        <v>320</v>
+        <v>3</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -6486,7 +6486,7 @@
         <v>27699922819</v>
       </c>
       <c r="D327">
-        <v>191</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -6500,7 +6500,7 @@
         <v>8586211830</v>
       </c>
       <c r="D328">
-        <v>1248</v>
+        <v>12</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -6514,7 +6514,7 @@
         <v>4095292500</v>
       </c>
       <c r="D329">
-        <v>2343</v>
+        <v>23</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -6528,7 +6528,7 @@
         <v>7631483371</v>
       </c>
       <c r="D330">
-        <v>1093</v>
+        <v>10</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -6542,7 +6542,7 @@
         <v>29064096758</v>
       </c>
       <c r="D331">
-        <v>334</v>
+        <v>3</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -6556,7 +6556,7 @@
         <v>152892371385</v>
       </c>
       <c r="D332">
-        <v>257</v>
+        <v>2</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -6570,7 +6570,7 @@
         <v>36750103245</v>
       </c>
       <c r="D333">
-        <v>427</v>
+        <v>4</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -6584,7 +6584,7 @@
         <v>159673551791</v>
       </c>
       <c r="D334">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -6598,7 +6598,7 @@
         <v>10965627234</v>
       </c>
       <c r="D335">
-        <v>733</v>
+        <v>7</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -6612,7 +6612,7 @@
         <v>198868800000</v>
       </c>
       <c r="D336">
-        <v>155</v>
+        <v>1</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -6626,7 +6626,7 @@
         <v>12352934758</v>
       </c>
       <c r="D337">
-        <v>915</v>
+        <v>9</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -6640,7 +6640,7 @@
         <v>10068164861</v>
       </c>
       <c r="D338">
-        <v>707</v>
+        <v>7</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -6654,7 +6654,7 @@
         <v>70548420829</v>
       </c>
       <c r="D339">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -6668,7 +6668,7 @@
         <v>9054154305</v>
       </c>
       <c r="D340">
-        <v>859</v>
+        <v>8</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -6682,7 +6682,7 @@
         <v>94173730000</v>
       </c>
       <c r="D341">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -6696,7 +6696,7 @@
         <v>8254666065</v>
       </c>
       <c r="D342">
-        <v>552</v>
+        <v>5</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -6710,7 +6710,7 @@
         <v>54278220915</v>
       </c>
       <c r="D343">
-        <v>83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -6724,7 +6724,7 @@
         <v>14812045359</v>
       </c>
       <c r="D344">
-        <v>288</v>
+        <v>2</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -6738,7 +6738,7 @@
         <v>20226741065</v>
       </c>
       <c r="D345">
-        <v>204</v>
+        <v>2</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -6752,7 +6752,7 @@
         <v>43632954197</v>
       </c>
       <c r="D346">
-        <v>116</v>
+        <v>1</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -6766,7 +6766,7 @@
         <v>566823600000</v>
       </c>
       <c r="D347">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -6780,7 +6780,7 @@
         <v>16493844972</v>
       </c>
       <c r="D348">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -6794,7 +6794,7 @@
         <v>6208136000</v>
       </c>
       <c r="D349">
-        <v>1319</v>
+        <v>13</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -6808,7 +6808,7 @@
         <v>11029012592</v>
       </c>
       <c r="D350">
-        <v>1024</v>
+        <v>10</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -6822,7 +6822,7 @@
         <v>11064229004</v>
       </c>
       <c r="D351">
-        <v>1034</v>
+        <v>10</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -6836,7 +6836,7 @@
         <v>41643016370</v>
       </c>
       <c r="D352">
-        <v>298</v>
+        <v>2</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -6850,7 +6850,7 @@
         <v>39465140195</v>
       </c>
       <c r="D353">
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -6864,7 +6864,7 @@
         <v>31139274172</v>
       </c>
       <c r="D354">
-        <v>284</v>
+        <v>2</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -6878,7 +6878,7 @@
         <v>18898964502</v>
       </c>
       <c r="D355">
-        <v>212</v>
+        <v>2</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -6892,7 +6892,7 @@
         <v>238186990020</v>
       </c>
       <c r="D356">
-        <v>224</v>
+        <v>2</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -6906,7 +6906,7 @@
         <v>53892251831</v>
       </c>
       <c r="D357">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -6920,7 +6920,7 @@
         <v>34965198173</v>
       </c>
       <c r="D358">
-        <v>234</v>
+        <v>2</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -6934,7 +6934,7 @@
         <v>57170699972</v>
       </c>
       <c r="D359">
-        <v>314</v>
+        <v>3</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -6948,7 +6948,7 @@
         <v>19206518080</v>
       </c>
       <c r="D360">
-        <v>61</v>
+        <v>0</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -6962,7 +6962,7 @@
         <v>41536560326</v>
       </c>
       <c r="D361">
-        <v>171</v>
+        <v>1</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -6976,7 +6976,7 @@
         <v>8371850392</v>
       </c>
       <c r="D362">
-        <v>1020</v>
+        <v>10</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -6990,7 +6990,7 @@
         <v>26051269043</v>
       </c>
       <c r="D363">
-        <v>264</v>
+        <v>2</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -7004,7 +7004,7 @@
         <v>14243684359</v>
       </c>
       <c r="D364">
-        <v>760</v>
+        <v>7</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -7018,7 +7018,7 @@
         <v>30815136189</v>
       </c>
       <c r="D365">
-        <v>320</v>
+        <v>3</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -7032,7 +7032,7 @@
         <v>242490597876</v>
       </c>
       <c r="D366">
-        <v>112</v>
+        <v>1</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -7046,7 +7046,7 @@
         <v>243168785743</v>
       </c>
       <c r="D367">
-        <v>457</v>
+        <v>4</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -7060,7 +7060,7 @@
         <v>22513263508</v>
       </c>
       <c r="D368">
-        <v>215</v>
+        <v>2</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -7074,7 +7074,7 @@
         <v>327826663580</v>
       </c>
       <c r="D369">
-        <v>142</v>
+        <v>1</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -7088,7 +7088,7 @@
         <v>83056496316</v>
       </c>
       <c r="D370">
-        <v>139</v>
+        <v>1</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -7102,7 +7102,7 @@
         <v>46324559395</v>
       </c>
       <c r="D371">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -7116,7 +7116,7 @@
         <v>12800361297</v>
       </c>
       <c r="D372">
-        <v>348</v>
+        <v>3</v>
       </c>
     </row>
     <row r="373" spans="1:4">
@@ -7130,7 +7130,7 @@
         <v>13195416848</v>
       </c>
       <c r="D373">
-        <v>138</v>
+        <v>1</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -7144,7 +7144,7 @@
         <v>17081886342</v>
       </c>
       <c r="D374">
-        <v>146</v>
+        <v>1</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -7158,7 +7158,7 @@
         <v>117720210925</v>
       </c>
       <c r="D375">
-        <v>155</v>
+        <v>1</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -7172,7 +7172,7 @@
         <v>156740955059</v>
       </c>
       <c r="D376">
-        <v>195</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -7186,7 +7186,7 @@
         <v>64531045280</v>
       </c>
       <c r="D377">
-        <v>123</v>
+        <v>1</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -7200,7 +7200,7 @@
         <v>9364891293</v>
       </c>
       <c r="D378">
-        <v>347</v>
+        <v>3</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -7214,7 +7214,7 @@
         <v>8445916154</v>
       </c>
       <c r="D379">
-        <v>265</v>
+        <v>2</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -7228,7 +7228,7 @@
         <v>30652272725</v>
       </c>
       <c r="D380">
-        <v>151</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -7242,7 +7242,7 @@
         <v>21117608385</v>
       </c>
       <c r="D381">
-        <v>690</v>
+        <v>6</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -7256,7 +7256,7 @@
         <v>4820102907</v>
       </c>
       <c r="D382">
-        <v>553</v>
+        <v>5</v>
       </c>
     </row>
     <row r="383" spans="1:4">
@@ -7270,7 +7270,7 @@
         <v>38673120000</v>
       </c>
       <c r="D383">
-        <v>190</v>
+        <v>1</v>
       </c>
     </row>
     <row r="384" spans="1:4">
@@ -7284,7 +7284,7 @@
         <v>52851347333</v>
       </c>
       <c r="D384">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="385" spans="1:4">
@@ -7298,7 +7298,7 @@
         <v>50406225516</v>
       </c>
       <c r="D385">
-        <v>185</v>
+        <v>1</v>
       </c>
     </row>
     <row r="386" spans="1:4">
@@ -7312,7 +7312,7 @@
         <v>5302917748</v>
       </c>
       <c r="D386">
-        <v>236</v>
+        <v>2</v>
       </c>
     </row>
     <row r="387" spans="1:4">
@@ -7326,7 +7326,7 @@
         <v>22292580336</v>
       </c>
       <c r="D387">
-        <v>126</v>
+        <v>1</v>
       </c>
     </row>
     <row r="388" spans="1:4">
@@ -7340,7 +7340,7 @@
         <v>53448739787</v>
       </c>
       <c r="D388">
-        <v>89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="389" spans="1:4">
@@ -7354,7 +7354,7 @@
         <v>88819560600</v>
       </c>
       <c r="D389">
-        <v>254</v>
+        <v>2</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -7368,7 +7368,7 @@
         <v>148373050000</v>
       </c>
       <c r="D390">
-        <v>148</v>
+        <v>1</v>
       </c>
     </row>
     <row r="391" spans="1:4">
@@ -7382,7 +7382,7 @@
         <v>10515337137</v>
       </c>
       <c r="D391">
-        <v>188</v>
+        <v>1</v>
       </c>
     </row>
     <row r="392" spans="1:4">
@@ -7396,7 +7396,7 @@
         <v>19330037636</v>
       </c>
       <c r="D392">
-        <v>261</v>
+        <v>2</v>
       </c>
     </row>
     <row r="393" spans="1:4">
@@ -7410,7 +7410,7 @@
         <v>15057780622</v>
       </c>
       <c r="D393">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="394" spans="1:4">
@@ -7424,7 +7424,7 @@
         <v>11157201344</v>
       </c>
       <c r="D394">
-        <v>303</v>
+        <v>3</v>
       </c>
     </row>
     <row r="395" spans="1:4">
@@ -7438,7 +7438,7 @@
         <v>80888557226</v>
       </c>
       <c r="D395">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="396" spans="1:4">
@@ -7452,7 +7452,7 @@
         <v>22333249983</v>
       </c>
       <c r="D396">
-        <v>828</v>
+        <v>8</v>
       </c>
     </row>
     <row r="397" spans="1:4">
@@ -7466,7 +7466,7 @@
         <v>9160531394</v>
       </c>
       <c r="D397">
-        <v>234</v>
+        <v>2</v>
       </c>
     </row>
     <row r="398" spans="1:4">
@@ -7480,7 +7480,7 @@
         <v>24522078835</v>
       </c>
       <c r="D398">
-        <v>173</v>
+        <v>1</v>
       </c>
     </row>
     <row r="399" spans="1:4">
@@ -7494,7 +7494,7 @@
         <v>8379641400</v>
       </c>
       <c r="D399">
-        <v>160</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400" spans="1:4">
@@ -7508,7 +7508,7 @@
         <v>31567894665</v>
       </c>
       <c r="D400">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="401" spans="1:4">
@@ -7522,7 +7522,7 @@
         <v>34210908328</v>
       </c>
       <c r="D401">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="402" spans="1:4">
@@ -7536,7 +7536,7 @@
         <v>17684685177</v>
       </c>
       <c r="D402">
-        <v>551</v>
+        <v>5</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -7550,7 +7550,7 @@
         <v>44710485446</v>
       </c>
       <c r="D403">
-        <v>46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -7564,7 +7564,7 @@
         <v>40167434490</v>
       </c>
       <c r="D404">
-        <v>169</v>
+        <v>1</v>
       </c>
     </row>
     <row r="405" spans="1:4">
@@ -7578,7 +7578,7 @@
         <v>39756077758</v>
       </c>
       <c r="D405">
-        <v>157</v>
+        <v>1</v>
       </c>
     </row>
     <row r="406" spans="1:4">
@@ -7592,7 +7592,7 @@
         <v>148634292093</v>
       </c>
       <c r="D406">
-        <v>195</v>
+        <v>1</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -7606,7 +7606,7 @@
         <v>31167491510</v>
       </c>
       <c r="D407">
-        <v>68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="408" spans="1:4">
@@ -7620,7 +7620,7 @@
         <v>125273700000</v>
       </c>
       <c r="D408">
-        <v>181</v>
+        <v>1</v>
       </c>
     </row>
     <row r="409" spans="1:4">
@@ -7634,7 +7634,7 @@
         <v>146139260085</v>
       </c>
       <c r="D409">
-        <v>246</v>
+        <v>2</v>
       </c>
     </row>
     <row r="410" spans="1:4">
@@ -7648,7 +7648,7 @@
         <v>7332689790</v>
       </c>
       <c r="D410">
-        <v>390</v>
+        <v>3</v>
       </c>
     </row>
     <row r="411" spans="1:4">
@@ -7662,7 +7662,7 @@
         <v>60289715732</v>
       </c>
       <c r="D411">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412" spans="1:4">
@@ -7676,7 +7676,7 @@
         <v>18721231277</v>
       </c>
       <c r="D412">
-        <v>62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="413" spans="1:4">
@@ -7690,7 +7690,7 @@
         <v>15633028085</v>
       </c>
       <c r="D413">
-        <v>134</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414" spans="1:4">
@@ -7704,7 +7704,7 @@
         <v>79516353667</v>
       </c>
       <c r="D414">
-        <v>353</v>
+        <v>3</v>
       </c>
     </row>
     <row r="415" spans="1:4">
@@ -7718,7 +7718,7 @@
         <v>2581646287</v>
       </c>
       <c r="D415">
-        <v>493</v>
+        <v>4</v>
       </c>
     </row>
     <row r="416" spans="1:4">
@@ -7732,7 +7732,7 @@
         <v>13491178925</v>
       </c>
       <c r="D416">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="417" spans="1:4">
@@ -7746,7 +7746,7 @@
         <v>57839276779</v>
       </c>
       <c r="D417">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="418" spans="1:4">
@@ -7760,7 +7760,7 @@
         <v>72690684726</v>
       </c>
       <c r="D418">
-        <v>296</v>
+        <v>2</v>
       </c>
     </row>
     <row r="419" spans="1:4">
@@ -7774,7 +7774,7 @@
         <v>41038235686</v>
       </c>
       <c r="D419">
-        <v>157</v>
+        <v>1</v>
       </c>
     </row>
     <row r="420" spans="1:4">
@@ -7788,7 +7788,7 @@
         <v>122400810000</v>
       </c>
       <c r="D420">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="421" spans="1:4">
@@ -7802,7 +7802,7 @@
         <v>49787261366</v>
       </c>
       <c r="D421">
-        <v>125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="422" spans="1:4">
@@ -7816,7 +7816,7 @@
         <v>19671226692</v>
       </c>
       <c r="D422">
-        <v>99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="423" spans="1:4">
@@ -7830,7 +7830,7 @@
         <v>34532737234</v>
       </c>
       <c r="D423">
-        <v>210</v>
+        <v>2</v>
       </c>
     </row>
     <row r="424" spans="1:4">
@@ -7844,7 +7844,7 @@
         <v>15024457200</v>
       </c>
       <c r="D424">
-        <v>275</v>
+        <v>2</v>
       </c>
     </row>
     <row r="425" spans="1:4">
@@ -7858,7 +7858,7 @@
         <v>41489959489</v>
       </c>
       <c r="D425">
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="426" spans="1:4">
@@ -7872,7 +7872,7 @@
         <v>13601767805</v>
       </c>
       <c r="D426">
-        <v>215</v>
+        <v>2</v>
       </c>
     </row>
     <row r="427" spans="1:4">
@@ -7886,7 +7886,7 @@
         <v>19351925958</v>
       </c>
       <c r="D427">
-        <v>162</v>
+        <v>1</v>
       </c>
     </row>
     <row r="428" spans="1:4">
@@ -7900,7 +7900,7 @@
         <v>16449267536</v>
       </c>
       <c r="D428">
-        <v>542</v>
+        <v>5</v>
       </c>
     </row>
     <row r="429" spans="1:4">
@@ -7914,7 +7914,7 @@
         <v>100389891565</v>
       </c>
       <c r="D429">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="430" spans="1:4">
@@ -7928,7 +7928,7 @@
         <v>39278398990</v>
       </c>
       <c r="D430">
-        <v>255</v>
+        <v>2</v>
       </c>
     </row>
     <row r="431" spans="1:4">
@@ -7942,7 +7942,7 @@
         <v>137252500000</v>
       </c>
       <c r="D431">
-        <v>1028</v>
+        <v>10</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -7956,7 +7956,7 @@
         <v>761570619</v>
       </c>
       <c r="D432">
-        <v>378</v>
+        <v>3</v>
       </c>
     </row>
     <row r="433" spans="1:4">
@@ -7970,7 +7970,7 @@
         <v>41940048842</v>
       </c>
       <c r="D433">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="434" spans="1:4">
@@ -7984,7 +7984,7 @@
         <v>20925130759</v>
       </c>
       <c r="D434">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="435" spans="1:4">
@@ -7998,7 +7998,7 @@
         <v>41936830752</v>
       </c>
       <c r="D435">
-        <v>149</v>
+        <v>1</v>
       </c>
     </row>
     <row r="436" spans="1:4">
@@ -8012,7 +8012,7 @@
         <v>64878871483</v>
       </c>
       <c r="D436">
-        <v>404</v>
+        <v>4</v>
       </c>
     </row>
     <row r="437" spans="1:4">
@@ -8026,7 +8026,7 @@
         <v>11593863539</v>
       </c>
       <c r="D437">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="438" spans="1:4">
@@ -8040,7 +8040,7 @@
         <v>81015428133</v>
       </c>
       <c r="D438">
-        <v>112</v>
+        <v>1</v>
       </c>
     </row>
     <row r="439" spans="1:4">
@@ -8054,7 +8054,7 @@
         <v>15960711882</v>
       </c>
       <c r="D439">
-        <v>150</v>
+        <v>1</v>
       </c>
     </row>
     <row r="440" spans="1:4">
@@ -8068,7 +8068,7 @@
         <v>93191409617</v>
       </c>
       <c r="D440">
-        <v>245</v>
+        <v>2</v>
       </c>
     </row>
     <row r="441" spans="1:4">
@@ -8082,7 +8082,7 @@
         <v>222308207574</v>
       </c>
       <c r="D441">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="442" spans="1:4">
@@ -8096,7 +8096,7 @@
         <v>183574942472</v>
       </c>
       <c r="D442">
-        <v>134</v>
+        <v>1</v>
       </c>
     </row>
     <row r="443" spans="1:4">
@@ -8110,7 +8110,7 @@
         <v>10932414226</v>
       </c>
       <c r="D443">
-        <v>436</v>
+        <v>4</v>
       </c>
     </row>
     <row r="444" spans="1:4">
@@ -8124,7 +8124,7 @@
         <v>27269411008</v>
       </c>
       <c r="D444">
-        <v>162</v>
+        <v>1</v>
       </c>
     </row>
     <row r="445" spans="1:4">
@@ -8138,7 +8138,7 @@
         <v>43405848581</v>
       </c>
       <c r="D445">
-        <v>106</v>
+        <v>1</v>
       </c>
     </row>
     <row r="446" spans="1:4">
@@ -8152,7 +8152,7 @@
         <v>26468098134</v>
       </c>
       <c r="D446">
-        <v>82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="447" spans="1:4">
@@ -8166,7 +8166,7 @@
         <v>22027337500</v>
       </c>
       <c r="D447">
-        <v>323</v>
+        <v>3</v>
       </c>
     </row>
     <row r="448" spans="1:4">
@@ -8180,7 +8180,7 @@
         <v>43108919665</v>
       </c>
       <c r="D448">
-        <v>105</v>
+        <v>1</v>
       </c>
     </row>
     <row r="449" spans="1:4">
@@ -8194,7 +8194,7 @@
         <v>19557811638</v>
       </c>
       <c r="D449">
-        <v>170</v>
+        <v>1</v>
       </c>
     </row>
     <row r="450" spans="1:4">
@@ -8208,7 +8208,7 @@
         <v>41093718362</v>
       </c>
       <c r="D450">
-        <v>368</v>
+        <v>3</v>
       </c>
     </row>
     <row r="451" spans="1:4">
@@ -8222,7 +8222,7 @@
         <v>161757734408</v>
       </c>
       <c r="D451">
-        <v>110</v>
+        <v>1</v>
       </c>
     </row>
     <row r="452" spans="1:4">
@@ -8236,7 +8236,7 @@
         <v>15595228958</v>
       </c>
       <c r="D452">
-        <v>265</v>
+        <v>2</v>
       </c>
     </row>
     <row r="453" spans="1:4">
@@ -8250,7 +8250,7 @@
         <v>13856508857</v>
       </c>
       <c r="D453">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="454" spans="1:4">
@@ -8264,7 +8264,7 @@
         <v>4163685725</v>
       </c>
       <c r="D454">
-        <v>2067</v>
+        <v>20</v>
       </c>
     </row>
     <row r="455" spans="1:4">
@@ -8278,7 +8278,7 @@
         <v>4129270564</v>
       </c>
       <c r="D455">
-        <v>1833</v>
+        <v>18</v>
       </c>
     </row>
     <row r="456" spans="1:4">
@@ -8292,7 +8292,7 @@
         <v>16307827877</v>
       </c>
       <c r="D456">
-        <v>396</v>
+        <v>3</v>
       </c>
     </row>
     <row r="457" spans="1:4">
@@ -8306,7 +8306,7 @@
         <v>14655890936</v>
       </c>
       <c r="D457">
-        <v>439</v>
+        <v>4</v>
       </c>
     </row>
     <row r="458" spans="1:4">
@@ -8320,7 +8320,7 @@
         <v>10809813131</v>
       </c>
       <c r="D458">
-        <v>133</v>
+        <v>1</v>
       </c>
     </row>
     <row r="459" spans="1:4">
@@ -8334,7 +8334,7 @@
         <v>26791778778</v>
       </c>
       <c r="D459">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="460" spans="1:4">
@@ -8348,7 +8348,7 @@
         <v>458998982111</v>
       </c>
       <c r="D460">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="461" spans="1:4">
@@ -8362,7 +8362,7 @@
         <v>8439072299</v>
       </c>
       <c r="D461">
-        <v>466</v>
+        <v>4</v>
       </c>
     </row>
     <row r="462" spans="1:4">
@@ -8376,7 +8376,7 @@
         <v>124872190488</v>
       </c>
       <c r="D462">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="463" spans="1:4">
@@ -8390,7 +8390,7 @@
         <v>161601308641</v>
       </c>
       <c r="D463">
-        <v>105</v>
+        <v>1</v>
       </c>
     </row>
     <row r="464" spans="1:4">
@@ -8404,7 +8404,7 @@
         <v>32620036583</v>
       </c>
       <c r="D464">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="465" spans="1:4">
@@ -8418,7 +8418,7 @@
         <v>72924216693</v>
       </c>
       <c r="D465">
-        <v>403</v>
+        <v>4</v>
       </c>
     </row>
     <row r="466" spans="1:4">
@@ -8432,7 +8432,7 @@
         <v>432753704051</v>
       </c>
       <c r="D466">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="467" spans="1:4">
@@ -8446,7 +8446,7 @@
         <v>16261898618</v>
       </c>
       <c r="D467">
-        <v>111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="468" spans="1:4">
@@ -8460,7 +8460,7 @@
         <v>10820206648</v>
       </c>
       <c r="D468">
-        <v>711</v>
+        <v>7</v>
       </c>
     </row>
     <row r="469" spans="1:4">
@@ -8474,7 +8474,7 @@
         <v>19317433987</v>
       </c>
       <c r="D469">
-        <v>669</v>
+        <v>6</v>
       </c>
     </row>
     <row r="470" spans="1:4">
@@ -8488,7 +8488,7 @@
         <v>52573809421</v>
       </c>
       <c r="D470">
-        <v>145</v>
+        <v>1</v>
       </c>
     </row>
     <row r="471" spans="1:4">
@@ -8502,7 +8502,7 @@
         <v>25976646960</v>
       </c>
       <c r="D471">
-        <v>101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="472" spans="1:4">
@@ -8516,7 +8516,7 @@
         <v>4482755905</v>
       </c>
       <c r="D472">
-        <v>847</v>
+        <v>8</v>
       </c>
     </row>
     <row r="473" spans="1:4">
@@ -8530,7 +8530,7 @@
         <v>27746350089</v>
       </c>
       <c r="D473">
-        <v>111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="474" spans="1:4">
@@ -8544,7 +8544,7 @@
         <v>22642994672</v>
       </c>
       <c r="D474">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="475" spans="1:4">
@@ -8558,7 +8558,7 @@
         <v>76686571285</v>
       </c>
       <c r="D475">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="476" spans="1:4">
@@ -8572,7 +8572,7 @@
         <v>20197749782</v>
       </c>
       <c r="D476">
-        <v>391</v>
+        <v>3</v>
       </c>
     </row>
     <row r="477" spans="1:4">
@@ -8586,7 +8586,7 @@
         <v>169588628510</v>
       </c>
       <c r="D477">
-        <v>490</v>
+        <v>4</v>
       </c>
     </row>
     <row r="478" spans="1:4">
@@ -8600,7 +8600,7 @@
         <v>19205246438</v>
       </c>
       <c r="D478">
-        <v>187</v>
+        <v>1</v>
       </c>
     </row>
     <row r="479" spans="1:4">
@@ -8614,7 +8614,7 @@
         <v>20014412018</v>
       </c>
       <c r="D479">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="480" spans="1:4">
@@ -8628,7 +8628,7 @@
         <v>31498629792</v>
       </c>
       <c r="D480">
-        <v>542</v>
+        <v>5</v>
       </c>
     </row>
     <row r="481" spans="1:4">
@@ -8642,7 +8642,7 @@
         <v>13944806369</v>
       </c>
       <c r="D481">
-        <v>453</v>
+        <v>4</v>
       </c>
     </row>
     <row r="482" spans="1:4">
@@ -8656,7 +8656,7 @@
         <v>29054674650</v>
       </c>
       <c r="D482">
-        <v>214</v>
+        <v>2</v>
       </c>
     </row>
     <row r="483" spans="1:4">
@@ -8670,7 +8670,7 @@
         <v>35779323891</v>
       </c>
       <c r="D483">
-        <v>261</v>
+        <v>2</v>
       </c>
     </row>
     <row r="484" spans="1:4">
@@ -8684,7 +8684,7 @@
         <v>182789248377</v>
       </c>
       <c r="D484">
-        <v>412</v>
+        <v>4</v>
       </c>
     </row>
     <row r="485" spans="1:4">
@@ -8698,7 +8698,7 @@
         <v>8054079855</v>
       </c>
       <c r="D485">
-        <v>133</v>
+        <v>1</v>
       </c>
     </row>
     <row r="486" spans="1:4">
@@ -8712,7 +8712,7 @@
         <v>28853787821</v>
       </c>
       <c r="D486">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="487" spans="1:4">
@@ -8726,7 +8726,7 @@
         <v>62096269927</v>
       </c>
       <c r="D487">
-        <v>130</v>
+        <v>1</v>
       </c>
     </row>
     <row r="488" spans="1:4">
@@ -8740,7 +8740,7 @@
         <v>39108708479</v>
       </c>
       <c r="D488">
-        <v>616</v>
+        <v>6</v>
       </c>
     </row>
     <row r="489" spans="1:4">
@@ -8754,7 +8754,7 @@
         <v>395269983915</v>
       </c>
       <c r="D489">
-        <v>135</v>
+        <v>1</v>
       </c>
     </row>
     <row r="490" spans="1:4">
@@ -8768,7 +8768,7 @@
         <v>17877161988</v>
       </c>
       <c r="D490">
-        <v>294</v>
+        <v>2</v>
       </c>
     </row>
     <row r="491" spans="1:4">
@@ -8782,7 +8782,7 @@
         <v>8502823034</v>
       </c>
       <c r="D491">
-        <v>593</v>
+        <v>5</v>
       </c>
     </row>
     <row r="492" spans="1:4">
@@ -8796,7 +8796,7 @@
         <v>20668529311</v>
       </c>
       <c r="D492">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="493" spans="1:4">
@@ -8810,7 +8810,7 @@
         <v>5479763766</v>
       </c>
       <c r="D493">
-        <v>1395</v>
+        <v>13</v>
       </c>
     </row>
     <row r="494" spans="1:4">
@@ -8824,7 +8824,7 @@
         <v>24174873450</v>
       </c>
       <c r="D494">
-        <v>602</v>
+        <v>6</v>
       </c>
     </row>
     <row r="495" spans="1:4">
@@ -8838,7 +8838,7 @@
         <v>12289992080</v>
       </c>
       <c r="D495">
-        <v>182</v>
+        <v>1</v>
       </c>
     </row>
     <row r="496" spans="1:4">
@@ -8852,7 +8852,7 @@
         <v>37158172878</v>
       </c>
       <c r="D496">
-        <v>291</v>
+        <v>2</v>
       </c>
     </row>
     <row r="497" spans="1:4">
@@ -8866,7 +8866,7 @@
         <v>48414620999</v>
       </c>
       <c r="D497">
-        <v>101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="498" spans="1:4">
@@ -8880,7 +8880,7 @@
         <v>478010317375</v>
       </c>
       <c r="D498">
-        <v>170</v>
+        <v>1</v>
       </c>
     </row>
     <row r="499" spans="1:4">
@@ -8894,7 +8894,7 @@
         <v>7863625909</v>
       </c>
       <c r="D499">
-        <v>541</v>
+        <v>5</v>
       </c>
     </row>
     <row r="500" spans="1:4">
@@ -8908,7 +8908,7 @@
         <v>2662361119</v>
       </c>
       <c r="D500">
-        <v>1157</v>
+        <v>11</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -8922,7 +8922,7 @@
         <v>19442298872</v>
       </c>
       <c r="D501">
-        <v>183</v>
+        <v>1</v>
       </c>
     </row>
     <row r="502" spans="1:4">
@@ -8936,7 +8936,7 @@
         <v>37089841316</v>
       </c>
       <c r="D502">
-        <v>150</v>
+        <v>1</v>
       </c>
     </row>
     <row r="503" spans="1:4">
@@ -8950,7 +8950,7 @@
         <v>26548426112</v>
       </c>
       <c r="D503">
-        <v>156</v>
+        <v>1</v>
       </c>
     </row>
     <row r="504" spans="1:4">
@@ -8964,7 +8964,7 @@
         <v>16883976542</v>
       </c>
       <c r="D504">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="505" spans="1:4">
@@ -8978,7 +8978,7 @@
         <v>7807054404</v>
       </c>
       <c r="D505">
-        <v>379</v>
+        <v>3</v>
       </c>
     </row>
     <row r="506" spans="1:4">
@@ -8992,7 +8992,7 @@
         <v>81571920565</v>
       </c>
       <c r="D506">
-        <v>113</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>